<commit_message>
Menu Dashboard - Remove
</commit_message>
<xml_diff>
--- a/Planejamento/Planejamento do Projto RH Verithus.xlsx
+++ b/Planejamento/Planejamento do Projto RH Verithus.xlsx
@@ -1124,11 +1124,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="75690592"/>
-        <c:axId val="75691152"/>
+        <c:axId val="106336928"/>
+        <c:axId val="153374384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75690592"/>
+        <c:axId val="106336928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,7 +1170,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75691152"/>
+        <c:crossAx val="153374384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1178,7 +1178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75691152"/>
+        <c:axId val="153374384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1228,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75690592"/>
+        <c:crossAx val="106336928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1953,11 +1953,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="75693952"/>
-        <c:axId val="75694512"/>
+        <c:axId val="153377184"/>
+        <c:axId val="153377744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75693952"/>
+        <c:axId val="153377184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,7 +2000,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75694512"/>
+        <c:crossAx val="153377744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2008,7 +2008,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75694512"/>
+        <c:axId val="153377744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2059,7 +2059,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75693952"/>
+        <c:crossAx val="153377184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3247,8 +3247,8 @@
         <xdr:to>
           <xdr:col>20</xdr:col>
           <xdr:colOff>200025</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4380,13 +4380,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:CL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -4415,7 +4415,7 @@
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
     </row>
-    <row r="3" spans="2:90" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:90" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
@@ -4467,7 +4467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:90" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:90" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
@@ -4484,12 +4484,12 @@
       <c r="AX4" s="1"/>
       <c r="AY4" s="1"/>
     </row>
-    <row r="5" spans="2:90" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:90" hidden="1" x14ac:dyDescent="0.3">
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
     </row>
-    <row r="6" spans="2:90" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:90" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
@@ -4514,7 +4514,7 @@
       <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
     </row>
-    <row r="7" spans="2:90" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:90" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:90" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4997,10 +4997,10 @@
         <v>1</v>
       </c>
       <c r="H17" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>26</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="14" t="s">
         <v>27</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
         <v>28</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
         <v>29</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
         <v>30</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="14" t="s">
         <v>31</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
         <v>20</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="s">
         <v>34</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>35</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="14" t="s">
         <v>36</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>37</v>
       </c>
@@ -5388,10 +5388,10 @@
         <v>2</v>
       </c>
       <c r="H34" s="16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
         <v>41</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" ht="18.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="14" t="s">
         <v>42</v>
       </c>
@@ -5438,7 +5438,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C2:C36"/>
+  <autoFilter ref="C2:C36">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Rômulo"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B2:K4"/>
   </mergeCells>
@@ -5499,8 +5505,8 @@
                   <to>
                     <xdr:col>20</xdr:col>
                     <xdr:colOff>200025</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>257175</xdr:rowOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>228600</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>